<commit_message>
trying to tune using one exp point only
this is not the best way to tune, all experimental data should be used
in the tuning process
</commit_message>
<xml_diff>
--- a/Interleaved-Christian/evap_N_circ_cross_couter_flow/purdue_conf_results/tuning results/tuning.xlsx
+++ b/Interleaved-Christian/evap_N_circ_cross_couter_flow/purdue_conf_results/tuning results/tuning.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\AllFiles\Volumes\Macintosh HD 2\Google Dirve\Purdue\PhD\Conferences\Purdue Conference 2016\Interleaved paper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Desktop\Eclipse Mars\Test\Interleaved-Christian\evap_N_circ_cross_couter_flow\purdue_conf_results\tuning results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3225" windowWidth="18060" windowHeight="12615"/>
+    <workbookView xWindow="0" yWindow="3690" windowWidth="18060" windowHeight="12620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -702,6 +702,7 @@
         <c:axId val="413480576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="40"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1335,6 +1336,7 @@
         <c:axId val="413480576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="30"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -11426,6 +11428,7 @@
         <c:axId val="413479920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="40"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -15105,6 +15108,7 @@
         <c:axId val="413479920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="25"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -27442,16 +27446,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
-      <selection activeCell="D160" sqref="D160"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="P34" sqref="P34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>19</v>
       </c>
@@ -27462,7 +27466,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B2" s="2"/>
       <c r="C2" s="9" t="s">
         <v>11</v>
@@ -27473,7 +27477,7 @@
       </c>
       <c r="F2" s="9"/>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
@@ -27490,7 +27494,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
@@ -27515,7 +27519,7 @@
         <v>273.48409264899999</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
@@ -27540,7 +27544,7 @@
         <v>279.84003969999998</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
@@ -27565,7 +27569,7 @@
         <v>272.42508505500001</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B7" s="3" t="s">
         <v>3</v>
       </c>
@@ -27590,7 +27594,7 @@
         <v>271.73189943099999</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
@@ -27615,7 +27619,7 @@
         <v>273.90199685800002</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
@@ -27640,7 +27644,7 @@
         <v>291.31349307300002</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B10" s="3" t="s">
         <v>6</v>
       </c>
@@ -27665,7 +27669,7 @@
         <v>280.512807259</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B11" s="3" t="s">
         <v>7</v>
       </c>
@@ -27690,7 +27694,7 @@
         <v>281.69345509999999</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
         <v>13</v>
       </c>
@@ -27701,7 +27705,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B42" s="2"/>
       <c r="C42" s="7" t="s">
         <v>11</v>
@@ -27712,7 +27716,7 @@
       </c>
       <c r="F42" s="7"/>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B43" s="2" t="s">
         <v>8</v>
       </c>
@@ -27729,7 +27733,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B44" s="3" t="s">
         <v>0</v>
       </c>
@@ -27754,7 +27758,7 @@
         <v>282.53579549099999</v>
       </c>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B45" s="3" t="s">
         <v>1</v>
       </c>
@@ -27779,7 +27783,7 @@
         <v>287.22678368099997</v>
       </c>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B46" s="3" t="s">
         <v>2</v>
       </c>
@@ -27804,7 +27808,7 @@
         <v>281.39947752500001</v>
       </c>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B47" s="3" t="s">
         <v>3</v>
       </c>
@@ -27829,7 +27833,7 @@
         <v>280.68027500400001</v>
       </c>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B48" s="3" t="s">
         <v>4</v>
       </c>
@@ -27854,7 +27858,7 @@
         <v>287.78142040799997</v>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B49" s="3" t="s">
         <v>5</v>
       </c>
@@ -27879,7 +27883,7 @@
         <v>287.14147960299999</v>
       </c>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B50" s="3" t="s">
         <v>6</v>
       </c>
@@ -27904,7 +27908,7 @@
         <v>288.17359304500002</v>
       </c>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B51" s="3" t="s">
         <v>7</v>
       </c>
@@ -27929,7 +27933,7 @@
         <v>293.99959292800003</v>
       </c>
     </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B75" t="s">
         <v>15</v>
       </c>
@@ -27940,7 +27944,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B76" s="2"/>
       <c r="C76" s="9" t="s">
         <v>11</v>
@@ -27951,7 +27955,7 @@
       </c>
       <c r="F76" s="9"/>
     </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B77" s="2" t="s">
         <v>8</v>
       </c>
@@ -27968,7 +27972,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B78" s="3" t="s">
         <v>0</v>
       </c>
@@ -27993,7 +27997,7 @@
         <v>287.94273920000001</v>
       </c>
     </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B79" s="3" t="s">
         <v>1</v>
       </c>
@@ -28018,7 +28022,7 @@
         <v>291.43679889999999</v>
       </c>
     </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B80" s="3" t="s">
         <v>2</v>
       </c>
@@ -28043,7 +28047,7 @@
         <v>286.65107771100003</v>
       </c>
     </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B81" s="3" t="s">
         <v>3</v>
       </c>
@@ -28068,7 +28072,7 @@
         <v>285.95498780200001</v>
       </c>
     </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B82" s="3" t="s">
         <v>4</v>
       </c>
@@ -28093,7 +28097,7 @@
         <v>291.86677290799997</v>
       </c>
     </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B83" s="3" t="s">
         <v>5</v>
       </c>
@@ -28118,7 +28122,7 @@
         <v>291.98243839999998</v>
       </c>
     </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B84" s="3" t="s">
         <v>6</v>
       </c>
@@ -28143,7 +28147,7 @@
         <v>292.75474742699998</v>
       </c>
     </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B85" s="3" t="s">
         <v>7</v>
       </c>
@@ -28168,7 +28172,7 @@
         <v>297.63025575699999</v>
       </c>
     </row>
-    <row r="112" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B112" t="s">
         <v>22</v>
       </c>
@@ -28182,7 +28186,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="113" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B113" s="2"/>
       <c r="C113" s="9" t="s">
         <v>11</v>
@@ -28193,7 +28197,7 @@
       </c>
       <c r="F113" s="9"/>
     </row>
-    <row r="114" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B114" s="2" t="s">
         <v>8</v>
       </c>
@@ -28210,7 +28214,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="115" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B115" s="3" t="s">
         <v>0</v>
       </c>
@@ -28235,7 +28239,7 @@
         <v>285.55561594699998</v>
       </c>
     </row>
-    <row r="116" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B116" s="3" t="s">
         <v>1</v>
       </c>
@@ -28260,7 +28264,7 @@
         <v>289.56677980000001</v>
       </c>
     </row>
-    <row r="117" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B117" s="3" t="s">
         <v>2</v>
       </c>
@@ -28285,7 +28289,7 @@
         <v>284.3667734</v>
       </c>
     </row>
-    <row r="118" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B118" s="3" t="s">
         <v>3</v>
       </c>
@@ -28310,7 +28314,7 @@
         <v>283.65570179999997</v>
       </c>
     </row>
-    <row r="119" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B119" s="3" t="s">
         <v>4</v>
       </c>
@@ -28335,7 +28339,7 @@
         <v>290.06454120000001</v>
       </c>
     </row>
-    <row r="120" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B120" s="3" t="s">
         <v>5</v>
       </c>
@@ -28360,7 +28364,7 @@
         <v>289.86567389999999</v>
       </c>
     </row>
-    <row r="121" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B121" s="3" t="s">
         <v>6</v>
       </c>
@@ -28385,7 +28389,7 @@
         <v>290.73802396399998</v>
       </c>
     </row>
-    <row r="122" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B122" s="3" t="s">
         <v>7</v>
       </c>
@@ -28410,7 +28414,7 @@
         <v>296.03857561799998</v>
       </c>
     </row>
-    <row r="150" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B150" t="s">
         <v>24</v>
       </c>
@@ -28421,7 +28425,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="151" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B151" s="2"/>
       <c r="C151" s="9" t="s">
         <v>11</v>
@@ -28432,7 +28436,7 @@
       </c>
       <c r="F151" s="9"/>
     </row>
-    <row r="152" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B152" s="2" t="s">
         <v>8</v>
       </c>
@@ -28449,7 +28453,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="153" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B153" s="3" t="s">
         <v>0</v>
       </c>
@@ -28474,7 +28478,7 @@
         <v>283.62140290399998</v>
       </c>
     </row>
-    <row r="154" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B154" s="3" t="s">
         <v>1</v>
       </c>
@@ -28499,7 +28503,7 @@
         <v>287.98641140000001</v>
       </c>
     </row>
-    <row r="155" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B155" s="3" t="s">
         <v>2</v>
       </c>
@@ -28524,7 +28528,7 @@
         <v>282.46953000000002</v>
       </c>
     </row>
-    <row r="156" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B156" s="3" t="s">
         <v>3</v>
       </c>
@@ -28549,7 +28553,7 @@
         <v>281.75521229999998</v>
       </c>
     </row>
-    <row r="157" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B157" s="3" t="s">
         <v>4</v>
       </c>
@@ -28574,7 +28578,7 @@
         <v>288.54593399999999</v>
       </c>
     </row>
-    <row r="158" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B158" s="3" t="s">
         <v>5</v>
       </c>
@@ -28599,7 +28603,7 @@
         <v>288.12838420000003</v>
       </c>
     </row>
-    <row r="159" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B159" s="3" t="s">
         <v>6</v>
       </c>
@@ -28624,7 +28628,7 @@
         <v>289.09595109999998</v>
       </c>
     </row>
-    <row r="160" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B160" s="3" t="s">
         <v>7</v>
       </c>

</xml_diff>